<commit_message>
updated MDK-ARM project with buzzer, leds, buttons and oled showcase
</commit_message>
<xml_diff>
--- a/project/Keil_Project/MF-config/IO分配情况.xlsx
+++ b/project/Keil_Project/MF-config/IO分配情况.xlsx
@@ -562,17 +562,17 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PA13</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>OUTPUT</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RST_soft_I2C</t>
         </is>
       </c>
     </row>
@@ -594,17 +594,17 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PA14</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>OUTPUT</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>HV_PSU</t>
         </is>
       </c>
     </row>
@@ -658,17 +658,17 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PA8</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>INPUT</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GM_pulse</t>
         </is>
       </c>
     </row>
@@ -754,17 +754,17 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PB2</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>WKUP_WKUP2</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>POWER_button</t>
         </is>
       </c>
     </row>
@@ -786,17 +786,17 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PB3</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>OUTPUT</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>POWER_EN</t>
         </is>
       </c>
     </row>
@@ -818,17 +818,17 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PB8</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>INPUT</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>USB_sense</t>
         </is>
       </c>
     </row>
@@ -914,17 +914,17 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PB11</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>OUTPUT</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BUZZER</t>
         </is>
       </c>
     </row>
@@ -1138,17 +1138,17 @@
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PC8</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ADC_IN9</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BATT_ADC_IN9</t>
         </is>
       </c>
     </row>
@@ -1202,17 +1202,17 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PC10</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>INPUT</t>
         </is>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MENU_button</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>LED1_red</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>LED2_green</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SDA_soft_I2C</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SCL_soft_I2C</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reconfigred base project to use interrupts
</commit_message>
<xml_diff>
--- a/project/Keil_Project/MF-config/IO分配情况.xlsx
+++ b/project/Keil_Project/MF-config/IO分配情况.xlsx
@@ -604,7 +604,7 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>HV_PSU</t>
+          <t>HV_enable_OUT</t>
         </is>
       </c>
     </row>
@@ -663,12 +663,12 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>INPUT</t>
+          <t>EXTI2_Select0</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>GM_pulse</t>
+          <t>GM_pulse_IRQ</t>
         </is>
       </c>
     </row>
@@ -759,12 +759,12 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>WKUP_WKUP2</t>
+          <t>EXTI4_Select2</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>POWER_button</t>
+          <t>POWER_button_IRQ</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>POWER_EN</t>
+          <t>POWER_enable_OUT</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>INPUT</t>
+          <t>EXTI6_Select0</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>USB_sense</t>
+          <t>USB_sense_IRQ</t>
         </is>
       </c>
     </row>
@@ -1207,12 +1207,12 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>INPUT</t>
+          <t>EXTI10_Select2</t>
         </is>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>MENU_button</t>
+          <t>MENU_button_IRQ</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>LED1_red</t>
+          <t>LED1_red_OUT</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>LED2_green</t>
+          <t>LED2_green_OUT</t>
         </is>
       </c>
     </row>

</xml_diff>